<commit_message>
Committing Integration and Functional Test Scripts
</commit_message>
<xml_diff>
--- a/StoreAppAutomation/Files/Cart_Items_Details.xlsx
+++ b/StoreAppAutomation/Files/Cart_Items_Details.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" r:id="rId8" sheetId="32"/>
-    <sheet name="Sheet1" r:id="rId9" sheetId="33"/>
-    <sheet name="Sheet0" r:id="rId7" sheetId="34"/>
+    <sheet name="Sheet0" r:id="rId7" sheetId="43"/>
+    <sheet name="Sheet2" r:id="rId8" sheetId="44"/>
+    <sheet name="Sheet1" r:id="rId9" sheetId="45"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="11">
   <si>
     <t>Store Item Name</t>
   </si>
@@ -379,7 +379,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -425,7 +425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -437,7 +437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>